<commit_message>
DDL e DML feitos
</commit_message>
<xml_diff>
--- a/Modelos/SPMedicalGroup_Fisico.xlsx
+++ b/Modelos/SPMedicalGroup_Fisico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35834520898\Documents\SPMedical_Group\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDF462A4-95FB-4848-B705-C33C4CB18904}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCF146F-6FBC-4CB0-95F4-6C8355B71081}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{2F519E1E-DD12-4F57-B085-C5B26EB1E9D8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="108">
   <si>
     <t>tipoUsuario</t>
   </si>
@@ -325,6 +325,30 @@
   </si>
   <si>
     <t>adm123</t>
+  </si>
+  <si>
+    <t>Ricardo</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>Sandman</t>
+  </si>
+  <si>
+    <t>Keanus</t>
+  </si>
+  <si>
+    <t>Monique</t>
+  </si>
+  <si>
+    <t>Robertin</t>
+  </si>
+  <si>
+    <t>Livia</t>
+  </si>
+  <si>
+    <t>adm1</t>
   </si>
 </sst>
 </file>
@@ -506,81 +530,96 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="14" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="18" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="17" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="11" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="12" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="16" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="15" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="15" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="14" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="13" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="13" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="19" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="18" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="17" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="12" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="11" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="11" borderId="0" xfId="10" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="16" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="19" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -916,585 +955,593 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D5B10E-1BB4-49CE-B343-4C2B45057882}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="25"/>
+      <c r="D1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="G1" s="12" t="s">
+      <c r="E1" s="27"/>
+      <c r="G1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="L2" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="10">
         <v>1</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="21" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="L3" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="D7" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>15</v>
+      </c>
+      <c r="G9" s="12">
+        <v>1</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="12">
+        <v>2</v>
+      </c>
+      <c r="E10" s="12">
+        <v>2</v>
+      </c>
+      <c r="F10" s="12">
+        <v>17</v>
+      </c>
+      <c r="G10" s="12">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="12">
+        <v>3</v>
+      </c>
+      <c r="E11" s="12">
+        <v>3</v>
+      </c>
+      <c r="F11" s="12">
+        <v>16</v>
+      </c>
+      <c r="G11" s="12">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <v>5</v>
       </c>
-      <c r="D5" s="6">
+      <c r="B13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="14">
+        <v>1</v>
+      </c>
+      <c r="E15" s="14">
+        <v>4</v>
+      </c>
+      <c r="F15" s="15">
+        <v>31079</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="14">
+        <v>15150</v>
+      </c>
+      <c r="I15" s="14">
+        <v>4654654164</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>8</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="14">
+        <v>2</v>
+      </c>
+      <c r="E16" s="14">
+        <v>5</v>
+      </c>
+      <c r="F16" s="15">
+        <v>36648</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="14">
+        <v>6215654154</v>
+      </c>
+      <c r="I16" s="14">
+        <v>456456165</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="14">
         <v>3</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="E17" s="14">
         <v>6</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="D7" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="F17" s="15">
+        <v>33171</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="14">
+        <v>454561545</v>
+      </c>
+      <c r="I17" s="14">
+        <v>6456465465</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>10</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="14">
+        <v>4</v>
+      </c>
+      <c r="E18" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="F18" s="15">
+        <v>43195</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="14">
+        <v>564654654</v>
+      </c>
+      <c r="I18" s="14">
+        <v>456465465</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>11</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>12</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>13</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="F21" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>14</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="12">
         <v>1</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="17">
+      <c r="E22" s="12">
         <v>1</v>
       </c>
-      <c r="E9" s="17">
+      <c r="F22" s="12">
         <v>1</v>
       </c>
-      <c r="F9" s="17">
+      <c r="G22" s="12">
+        <v>3</v>
+      </c>
+      <c r="H22" s="16">
+        <v>44426</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <v>15</v>
       </c>
-      <c r="G9" s="17">
+      <c r="B23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="12">
+        <v>2</v>
+      </c>
+      <c r="E23" s="12">
+        <v>3</v>
+      </c>
+      <c r="F23" s="12">
+        <v>4</v>
+      </c>
+      <c r="G23" s="12">
         <v>1</v>
       </c>
-      <c r="H9" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="H23" s="16">
+        <v>44424</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>16</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="12">
+        <v>3</v>
+      </c>
+      <c r="E24" s="12">
         <v>2</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="17">
+      <c r="F24" s="12">
         <v>2</v>
       </c>
-      <c r="E10" s="17">
+      <c r="G24" s="12">
+        <v>3</v>
+      </c>
+      <c r="H24" s="16">
+        <v>44458</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>17</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="12">
+        <v>4</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1</v>
+      </c>
+      <c r="F25" s="12">
+        <v>3</v>
+      </c>
+      <c r="G25" s="12">
         <v>2</v>
       </c>
-      <c r="F10" s="17">
-        <v>17</v>
-      </c>
-      <c r="G10" s="17">
-        <v>1</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="17">
-        <v>3</v>
-      </c>
-      <c r="E11" s="17">
-        <v>3</v>
-      </c>
-      <c r="F11" s="17">
-        <v>16</v>
-      </c>
-      <c r="G11" s="17">
-        <v>1</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>6</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="20">
-        <v>1</v>
-      </c>
-      <c r="E15" s="20">
-        <v>4</v>
-      </c>
-      <c r="F15" s="21">
-        <v>31079</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="20">
-        <v>15150</v>
-      </c>
-      <c r="I15" s="20">
-        <v>4654654164</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="20">
-        <v>2</v>
-      </c>
-      <c r="E16" s="20">
-        <v>5</v>
-      </c>
-      <c r="F16" s="21">
-        <v>36648</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="20">
-        <v>6215654154</v>
-      </c>
-      <c r="I16" s="20">
-        <v>456456165</v>
-      </c>
-      <c r="J16" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="K16" s="20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="20">
-        <v>3</v>
-      </c>
-      <c r="E17" s="20">
-        <v>6</v>
-      </c>
-      <c r="F17" s="21">
-        <v>33171</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="20">
-        <v>454561545</v>
-      </c>
-      <c r="I17" s="20">
-        <v>6456465465</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="K17" s="20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="20">
-        <v>4</v>
-      </c>
-      <c r="E18" s="20">
-        <v>7</v>
-      </c>
-      <c r="F18" s="21">
-        <v>43195</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="20">
-        <v>564654654</v>
-      </c>
-      <c r="I18" s="20">
-        <v>456465465</v>
-      </c>
-      <c r="J18" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="K18" s="20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>11</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>12</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>13</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>14</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="17">
-        <v>1</v>
-      </c>
-      <c r="E22" s="17">
-        <v>1</v>
-      </c>
-      <c r="F22" s="17">
-        <v>1</v>
-      </c>
-      <c r="G22" s="17">
-        <v>3</v>
-      </c>
-      <c r="H22" s="23">
-        <v>44426</v>
-      </c>
-      <c r="I22" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>15</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="17">
-        <v>2</v>
-      </c>
-      <c r="E23" s="17">
-        <v>3</v>
-      </c>
-      <c r="F23" s="17">
-        <v>4</v>
-      </c>
-      <c r="G23" s="17">
-        <v>1</v>
-      </c>
-      <c r="H23" s="23">
-        <v>44424</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>16</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="17">
-        <v>3</v>
-      </c>
-      <c r="E24" s="17">
-        <v>2</v>
-      </c>
-      <c r="F24" s="17">
-        <v>2</v>
-      </c>
-      <c r="G24" s="17">
-        <v>3</v>
-      </c>
-      <c r="H24" s="23">
-        <v>44458</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>17</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="17">
-        <v>4</v>
-      </c>
-      <c r="E25" s="17">
-        <v>1</v>
-      </c>
-      <c r="F25" s="17">
-        <v>3</v>
-      </c>
-      <c r="G25" s="17">
-        <v>2</v>
-      </c>
-      <c r="H25" s="23">
+      <c r="H25" s="16">
         <v>44317</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I25" s="12" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1505,153 +1552,181 @@
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="E28" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="A29" s="10">
         <v>1</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="10">
         <v>2</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="E29" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
+      <c r="A30" s="10">
         <v>2</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="10">
         <v>2</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="E30" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
+      <c r="A31" s="10">
         <v>3</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="10">
         <v>2</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="E31" s="10" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
+      <c r="A32" s="10">
         <v>4</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="10">
         <v>3</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="E32" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
         <v>5</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="10">
         <v>3</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="E33" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
         <v>6</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="10">
         <v>3</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="E34" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
         <v>7</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="10">
         <v>3</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="E35" s="10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
         <v>8</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="10">
         <v>1</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="E36" s="10" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="D20:I20"/>
-    <mergeCell ref="A27:D27"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:K1"/>
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="D13:K13"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="G1:L1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C29" r:id="rId1" xr:uid="{83AFF6CF-109E-4A71-8172-5027B05E885D}"/>
-    <hyperlink ref="C30" r:id="rId2" xr:uid="{895895CD-0FD3-495C-B371-2A12380F0942}"/>
-    <hyperlink ref="C31" r:id="rId3" xr:uid="{834F5399-0887-4372-A5F0-C8E6FD0753D7}"/>
-    <hyperlink ref="C32" r:id="rId4" xr:uid="{56EC06DC-D702-49F8-B00A-65A6D81454EC}"/>
-    <hyperlink ref="C33" r:id="rId5" xr:uid="{FB462639-36BD-4D2D-A336-BB132F805515}"/>
-    <hyperlink ref="C34" r:id="rId6" xr:uid="{6F9F1EFE-8039-4050-8A20-36BD8DE939AD}"/>
-    <hyperlink ref="C35" r:id="rId7" xr:uid="{9011401B-6B99-4F4D-8EB1-93FBC67127FA}"/>
-    <hyperlink ref="C36" r:id="rId8" xr:uid="{4FFF0A90-965D-4427-8A85-9BB291E6DBD5}"/>
+    <hyperlink ref="D29" r:id="rId1" xr:uid="{83AFF6CF-109E-4A71-8172-5027B05E885D}"/>
+    <hyperlink ref="D30" r:id="rId2" xr:uid="{895895CD-0FD3-495C-B371-2A12380F0942}"/>
+    <hyperlink ref="D31" r:id="rId3" xr:uid="{834F5399-0887-4372-A5F0-C8E6FD0753D7}"/>
+    <hyperlink ref="D32" r:id="rId4" xr:uid="{56EC06DC-D702-49F8-B00A-65A6D81454EC}"/>
+    <hyperlink ref="D33" r:id="rId5" xr:uid="{FB462639-36BD-4D2D-A336-BB132F805515}"/>
+    <hyperlink ref="D34" r:id="rId6" xr:uid="{6F9F1EFE-8039-4050-8A20-36BD8DE939AD}"/>
+    <hyperlink ref="D35" r:id="rId7" xr:uid="{9011401B-6B99-4F4D-8EB1-93FBC67127FA}"/>
+    <hyperlink ref="D36" r:id="rId8" xr:uid="{4FFF0A90-965D-4427-8A85-9BB291E6DBD5}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>